<commit_message>
Excel file and report changes
</commit_message>
<xml_diff>
--- a/Resources/TestData.xlsx
+++ b/Resources/TestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{947E1E4E-DE43-4949-92EB-468710B066CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{F181294E-987E-48F9-9406-74E7E2643267}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="23304" windowHeight="13224" xr2:uid="{608866AC-74CC-4191-B744-0C917569FA43}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="23304" windowHeight="13224" xr2:uid="{608866AC-74CC-4191-B744-0C917569FA43}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>TestCase</t>
   </si>
@@ -424,7 +424,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -457,19 +457,16 @@
       <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" t="s">
         <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>

</xml_diff>